<commit_message>
Uploading results to compare testing to.
</commit_message>
<xml_diff>
--- a/tests/TestResults/obfuscated_tdm_param_checking_results_summary.xlsx
+++ b/tests/TestResults/obfuscated_tdm_param_checking_results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jamesson\Documents\GitHub\deck_themer_v2\tests\TestResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8189E32A-69D0-4A66-8482-4A8B5803BA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CBDF97-7BDD-4D4D-A150-B26EF6298C37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="36">
   <si>
     <t>tw</t>
   </si>
@@ -121,21 +121,31 @@
     <t>gamma = 1</t>
   </si>
   <si>
-    <t>Average Values Across All 3 Runs:</t>
+    <t>Average Values Across All 3 Runs, k0 = 2:</t>
   </si>
   <si>
-    <t>Standard Deviation of Values Across All 3 Runs:</t>
+    <t>Standard Deviation of Values Across All 3 Runs, k0 = 2:</t>
   </si>
   <si>
-    <t>Coefficient of Variation of Values Across All 3 Runs:</t>
+    <t>Coefficient of Variation of Values Across All 3 Runs, k0 = 2:</t>
+  </si>
+  <si>
+    <t>Average Values Across All 3 Runs, k0 = 9:</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Values Across All 3 Runs, k0 = 9:</t>
+  </si>
+  <si>
+    <t>Coefficient of Variation of Values Across All 3 Runs, k0 = 9:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -250,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -278,6 +288,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3256,11 +3270,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F127ECC-312A-41D1-BFD5-E73AE75AA02A}">
-  <dimension ref="A1:T53"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H68" sqref="H68"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5816,118 +5830,207 @@
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G51" s="12" t="s">
+      <c r="E51" s="12"/>
+      <c r="F51" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="12"/>
-      <c r="I51" s="12"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
       <c r="J51">
-        <f>AVERAGE(Table1[k])</f>
-        <v>17.270833333333332</v>
+        <v>11.875</v>
       </c>
       <c r="K51">
-        <f>AVERAGE(Table1[Live k])</f>
-        <v>14.166666666666666</v>
+        <v>9.4166666666666661</v>
       </c>
       <c r="L51">
-        <f>AVERAGE(Table1[Avg. LL])</f>
-        <v>-12.031093478524246</v>
+        <v>-12.167870479017138</v>
       </c>
       <c r="M51">
-        <f>AVERAGE(Table1[LL Std. Dev.])</f>
-        <v>1.6007275165138328E-2</v>
-      </c>
-      <c r="N51" s="2">
-        <f>AVERAGE(Table1[LL CV])</f>
-        <v>-1.3300753792051866E-3</v>
+        <v>1.5824739505218434E-2</v>
+      </c>
+      <c r="N51">
+        <v>-1.299338534486218E-3</v>
       </c>
       <c r="O51">
-        <f>AVERAGE(Table1[Perplexity])</f>
-        <v>167618.87208658096</v>
+        <v>190348.51506485025</v>
       </c>
       <c r="P51">
-        <f>AVERAGE(Table1[Coherence])</f>
-        <v>0.88453380100630741</v>
+        <v>0.91726521708941322</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F52" s="12" t="s">
+      <c r="E52" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
       <c r="J52">
-        <f>_xlfn.STDEV.P(Table1[k])</f>
-        <v>8.7695961122632227</v>
+        <v>2.7433632035635869</v>
       </c>
       <c r="K52">
-        <f>_xlfn.STDEV.P(Table1[Live k])</f>
-        <v>7.2495210569771817</v>
+        <v>2.1778557242286634</v>
       </c>
       <c r="L52">
-        <f>_xlfn.STDEV.P(Table1[Avg. LL])</f>
-        <v>0.14326625354293498</v>
+        <v>2.3839227858034856E-2</v>
       </c>
       <c r="M52">
-        <f>_xlfn.STDEV.P(Table1[LL Std. Dev.])</f>
-        <v>1.1305427585528553E-2</v>
-      </c>
-      <c r="N52" s="2">
-        <f>_xlfn.STDEV.P(Table1[LL CV])</f>
-        <v>9.4082970341264878E-4</v>
+        <v>1.0515126679311612E-2</v>
+      </c>
+      <c r="N52">
+        <v>8.6246493958625371E-4</v>
       </c>
       <c r="O52">
-        <f>_xlfn.STDEV.P(Table1[Perplexity])</f>
-        <v>23600.028825908594</v>
+        <v>3905.242226268118</v>
       </c>
       <c r="P52">
-        <f>_xlfn.STDEV.P(Table1[Coherence])</f>
-        <v>6.1097887765759334E-2</v>
+        <v>4.8923382458746757E-2</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
-      <c r="H53" s="12"/>
-      <c r="I53" s="12"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
       <c r="J53" s="11">
         <f>J52/J51</f>
-        <v>0.50776913557133263</v>
+        <v>0.23102005924745994</v>
       </c>
       <c r="K53" s="11">
         <f t="shared" ref="K53:P53" si="0">K52/K51</f>
-        <v>0.51173089813956574</v>
+        <v>0.23127671407738021</v>
       </c>
       <c r="L53" s="11">
         <f t="shared" si="0"/>
-        <v>-1.1907999368359014E-2</v>
+        <v>-1.9591947415239478E-3</v>
       </c>
       <c r="M53" s="11">
         <f t="shared" si="0"/>
-        <v>0.70626808553589671</v>
+        <v>0.66447391919747545</v>
       </c>
       <c r="N53" s="11">
         <f t="shared" si="0"/>
-        <v>-0.70735066457275575</v>
+        <v>-0.66377230929065612</v>
       </c>
       <c r="O53" s="11">
         <f t="shared" si="0"/>
-        <v>0.14079577396105111</v>
+        <v>2.0516273662222334E-2</v>
       </c>
       <c r="P53" s="11">
         <f t="shared" si="0"/>
-        <v>6.9073547778784841E-2</v>
+        <v>5.3336136100294099E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E55" s="12"/>
+      <c r="F55" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55">
+        <v>22.666666666666668</v>
+      </c>
+      <c r="K55">
+        <v>18.916666666666668</v>
+      </c>
+      <c r="L55">
+        <v>-11.89431647803135</v>
+      </c>
+      <c r="M55">
+        <v>1.6189810825058219E-2</v>
+      </c>
+      <c r="N55" s="2">
+        <v>-1.3608122239241549E-3</v>
+      </c>
+      <c r="O55">
+        <v>144889.22910831167</v>
+      </c>
+      <c r="P55">
+        <v>0.85180238492320193</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E56" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56">
+        <v>9.3837921735061656</v>
+      </c>
+      <c r="K56">
+        <v>7.4325672250949442</v>
+      </c>
+      <c r="L56">
+        <v>5.5373588432790583E-2</v>
+      </c>
+      <c r="M56">
+        <v>1.2041214978855094E-2</v>
+      </c>
+      <c r="N56" s="2">
+        <v>1.012218248395567E-3</v>
+      </c>
+      <c r="O56">
+        <v>8086.9317100137114</v>
+      </c>
+      <c r="P56">
+        <v>5.4126843895234325E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E57" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="11">
+        <f>J56/J55</f>
+        <v>0.41399083118409552</v>
+      </c>
+      <c r="K57" s="11">
+        <f t="shared" ref="K57:P57" si="1">K56/K55</f>
+        <v>0.39291104273629657</v>
+      </c>
+      <c r="L57" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.6554662081730288E-3</v>
+      </c>
+      <c r="M57" s="11">
+        <f t="shared" si="1"/>
+        <v>0.74375266696865761</v>
+      </c>
+      <c r="N57" s="11">
+        <f t="shared" si="1"/>
+        <v>-0.7438338887614101</v>
+      </c>
+      <c r="O57" s="14">
+        <f t="shared" si="1"/>
+        <v>5.5814581662024999E-2</v>
+      </c>
+      <c r="P57" s="14">
+        <f t="shared" si="1"/>
+        <v>6.3543898037001126E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="F52:I52"/>
+  <mergeCells count="6">
     <mergeCell ref="E53:I53"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="E52:I52"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="E56:I56"/>
+    <mergeCell ref="E57:I57"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>